<commit_message>
displaying players on squad page from database.
</commit_message>
<xml_diff>
--- a/Pseudo Code/manageTeam.xlsx
+++ b/Pseudo Code/manageTeam.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Pseudo Code</t>
   </si>
@@ -102,9 +102,6 @@
   </si>
   <si>
     <t>else</t>
-  </si>
-  <si>
-    <t>return true</t>
   </si>
   <si>
     <t>end if</t>
@@ -484,7 +481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
@@ -657,15 +654,15 @@
     <row r="29" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
@@ -677,12 +674,12 @@
     <row r="32" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B33" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -692,12 +689,12 @@
     </row>
     <row r="35" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B35" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B36" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -707,17 +704,17 @@
     </row>
     <row r="38" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B38" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B39" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B40" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>